<commit_message>
barely getting htmltext to work
</commit_message>
<xml_diff>
--- a/mom2e_insanity.xlsx
+++ b/mom2e_insanity.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trasa\OneDrive\Documents\games\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trasa\mom2e\insanity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="8_{95EEFAD5-14B6-451B-83E9-8347B48EB7B4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{26CEE128-E3A5-45A5-BF80-9A2B10D6B257}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FC9B60-BF9C-4F0D-AD65-089781D2C3E3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{3318FF81-56BE-4CC7-A916-502FDCE62A14}"/>
   </bookViews>
@@ -48,20 +48,10 @@
     <t xml:space="preserve">You must tell them to lay down their arms and allow the grace of God to purify their sins. </t>
   </si>
   <si>
-    <t xml:space="preserve">You do not win the game as normal. Instead, you win only if the investigation is complete and this card has been revealed.
-Miracle: At the start of the Investigator Phase, if you have a Light Source, a Bladed Weapon, and an Evidence Unique Item, and you are sharing a space with another investigator, you may reveal this card. That investigator may discard a Wounded or Insane condition. This miracle may only happen once per game.
-</t>
-  </si>
-  <si>
     <t>One of the Thousand</t>
   </si>
   <si>
     <t xml:space="preserve">He plots against you, and you are the only one who sees through his wicked lies and deception. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">You do not win the game as normal. Instead, you win only if the investigation is complete and this card has been revealed.
-Execution Attempt: At the start of the Investigator Phase, if you have a Bladed Weapon and you are in a space with exactly one other investigator, you may reveal this card. If that investigator is not Wounded, he becomes Wounded and discards all facedown Damage. If he is Wounded, that investigator is eliminated. The game does not end as a result of that investigator’s elimination. This execution attempt may only happen once per game.
-</t>
   </si>
   <si>
     <r>
@@ -111,11 +101,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">You do not win the game as normal. Instead, you only win if the investigation is complete and this card has been revealed.
-Conflagration: At the start of the Investigator Phase, if 6 or more rooms contain Fire, reveal this card. While this card is revealed, at the beginning of each Mythos phase, fire spreads twice.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">• Set Fire (Action): If you have a Light Source, place a Fire in your space or an adjacent space. Select the “Set Fire” option in the app.
 • Extinguish Fire (Action): Test Agility. For each success, discard Fire from your space or a space you move into later during the round. Doesn’t do Damage.
 • If group disagrees about how a fire should spread, a random investigator decides. Roll a die, draw cards, use an app, or do something else.
@@ -125,10 +110,6 @@
     <t>For The Greater Good</t>
   </si>
   <si>
-    <t>You do not win the game as normal. Instead, you win only if the investigation is complete and this card has been revealed.
-Martyrdom: After you have been eliminated, reveal this card. The game does not end as a result of your elimination.</t>
-  </si>
-  <si>
     <t>•	When eliminated, you drop all possessions onto your space and remove your figure from the board. You cannot take actions.
 •	Normally, eliminations cause the eliminated player to lose and the group to lose after the next Investigation phase. This card overrides that rule.</t>
   </si>
@@ -139,10 +120,6 @@
     <t>You know how to quiet the voices in your head, but a blood sacrifice will be required.</t>
   </si>
   <si>
-    <t>You do not win the game as normal. Instead, you win only if the investigation is complete and this card has been revealed.
-Bloodletting: At the start of the Investigator Phase, if you have a Bladed Weapon and there is at least one other investigator on your space, you may reveal this card and choose one investigator on your space. That investigator suffers one facedown Damage, and you discard one Horror. Other investigators within range flip one Horror.</t>
-  </si>
-  <si>
     <t>•	Steal (Action): Pick an investigator in your space. Pick Strength, Agility, or Observation. Each player rolls that test. For each net success over your opponent’s, you take one possession.
 •	“Within Range:” Means up to 3 spaces away. Cannot count through walls, doors, or impassable borders, unless an effect says otherwise.</t>
   </si>
@@ -202,10 +179,6 @@
     <t>There are more things in heaven and earth than are dreamt of in your philosophy.</t>
   </si>
   <si>
-    <t>You do not win the game as normal. Instead, you win if the investigation is complete and this card has been revealed.
-Burn the Evidence: At the start of the Investigator Phase, if you possess two Evidence Unique Items while standing on or adjacent to a space that contains Fire, you may reveal this card. Discard two Evidence Unique items from your inventory.</t>
-  </si>
-  <si>
     <t>•	Set Fire (Action): If you have a Light Source, place a Fire in your space or an adjacent space. Select the “Set Fire” option in the app.
 •	Steal (Action): Pick an investigator in your space. Pick Strength, Agility, or Observation. Each player rolls that test. For each net success over your opponent’s, you take one possession.</t>
   </si>
@@ -281,23 +254,54 @@
     <t>The Lurker at the Threshold has promised you great knowledge in exchange for a small price. You are ready to learn the first and last secret.</t>
   </si>
   <si>
+    <t>Even though you call them your "friends," why do you grin when they fall?</t>
+  </si>
+  <si>
+    <t>You have gazed too far into the abyss and fought too long with monsters. There is no room for you in the better world you fight to preserve. Best if you not live to see it.</t>
+  </si>
+  <si>
+    <t>They are laughing at your misfortune. You can tell. But they will not laugh for very much longer. . .</t>
+  </si>
+  <si>
+    <t>What's the point? None of this matters anyway.</t>
+  </si>
+  <si>
+    <t>You are suddenly stricken with the sense that your life up to this point has been not only boring but pointless. Life is too short to not experience as much of the world as possible.</t>
+  </si>
+  <si>
     <t>You do not win the game as normal. Instead, you win only if the investigation is complete and this card has been revealed.
-Horrific Offering: At the start of the Investigator Phase, if you have a Bladed Weapon and 1 or more Spells, and there is at least one other investigator on your space, you may reveal this card and choose one investigator on your space. That investigator suffers one Damage and becomes Insane. (If the investigator was already Insane, the investigator is eliminated as normal.) This offering may only happen once per game.</t>
-  </si>
-  <si>
-    <t>Even though you call them your "friends," why do you grin when they fall?</t>
-  </si>
-  <si>
-    <t>You have gazed too far into the abyss and fought too long with monsters. There is no room for you in the better world you fight to preserve. Best if you not live to see it.</t>
-  </si>
-  <si>
-    <t>They are laughing at your misfortune. You can tell. But they will not laugh for very much longer. . .</t>
-  </si>
-  <si>
-    <t>What's the point? None of this matters anyway.</t>
-  </si>
-  <si>
-    <t>You are suddenly stricken with the sense that your life up to this point has been not only boring but pointless. Life is too short to not experience as much of the world as possible.</t>
+&lt;p&gt;
+&lt;b&gt;Execution Attempt:&lt;/b&gt; At the start of the Investigator Phase, if you have a Bladed Weapon and you are in a space with exactly one other investigator, you may reveal this card. If that investigator is not Wounded, he becomes Wounded and discards all facedown Damage. If he is Wounded, that investigator is eliminated. The game does not end as a result of that investigator’s elimination. This execution attempt may only happen once per game.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You do not win the game as normal. Instead, you only win if the investigation is complete and this card has been revealed.
+&lt;p&gt;
+&lt;b&gt;Conflagration:&lt;/b&gt; At the start of the Investigator Phase, if 6 or more rooms contain Fire, reveal this card. While this card is revealed, at the beginning of each Mythos phase, fire spreads twice.
+</t>
+  </si>
+  <si>
+    <t>You do not win the game as normal. Instead, you win only if the investigation is complete and this card has been revealed.
+&lt;p&gt;
+&lt;b&gt;Martyrdom:&lt;/b&gt; After you have been eliminated, reveal this card. The game does not end as a result of your elimination.</t>
+  </si>
+  <si>
+    <t>You do not win the game as normal. Instead, you win only if the investigation is complete and this card has been revealed.
+&lt;p&gt;
+&lt;b&gt;Bloodletting:&lt;/b&gt; At the start of the Investigator Phase, if you have a Bladed Weapon and there is at least one other investigator on your space, you may reveal this card and choose one investigator on your space. That investigator suffers one facedown Damage, and you discard one Horror. Other investigators within range flip one Horror.</t>
+  </si>
+  <si>
+    <t>You do not win the game as normal. Instead, you win if the investigation is complete and this card has been revealed.
+&lt;p&gt;
+&lt;b&gt;Burn the Evidence:&lt;/b&gt; At the start of the Investigator Phase, if you possess two Evidence Unique Items while standing on or adjacent to a space that contains Fire, you may reveal this card. Discard two Evidence Unique items from your inventory.</t>
+  </si>
+  <si>
+    <t>You do not win the game as normal. Instead, you win only if the investigation is complete and this card has been revealed.
+&lt;p&gt;
+&lt;b&gt;Horrific Offering:&lt;/b&gt; At the start of the Investigator Phase, if you have a Bladed Weapon and 1 or more Spells, and there is at least one other investigator on your space, you may reveal this card and choose one investigator on your space. That investigator suffers one Damage and becomes Insane. (If the investigator was already Insane, the investigator is eliminated as normal.) This offering may only happen once per game.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You do not win the game as normal. Instead, you win only if the investigation is complete and this card has been revealed.
+&lt;/p&gt;&lt;b&gt;Miracle:&lt;/b&gt; At the start of the Investigator Phase, if you have a Light Source, a Bladed Weapon, and an Evidence Unique Item, and you are sharing a space with another investigator, you may reveal this card. That investigator may discard a Wounded or Insane condition. This miracle may only happen once per game.</t>
   </si>
 </sst>
 </file>
@@ -744,8 +748,8 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,7 +779,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -786,310 +790,310 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="B3" s="2">
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2">
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2">
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B8" s="2">
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B14" s="2">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B15" s="2">
         <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B16" s="2">
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B17" s="2">
         <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B19" s="2">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B20" s="2">
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first version seems to look good
</commit_message>
<xml_diff>
--- a/mom2e_insanity.xlsx
+++ b/mom2e_insanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trasa\mom2e\insanity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FC9B60-BF9C-4F0D-AD65-089781D2C3E3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF744E8F-3018-4CFE-9D53-699DFFABF3BA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{3318FF81-56BE-4CC7-A916-502FDCE62A14}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="75">
   <si>
     <t>Name</t>
   </si>
@@ -52,21 +52,6 @@
   </si>
   <si>
     <t xml:space="preserve">He plots against you, and you are the only one who sees through his wicked lies and deception. </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Steal (Action): </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Pick an investigator in your space. Pick Strength, Agility, or Observation. Each player rolls that test. For each net success over your opponent’s, you take one possession.</t>
-    </r>
   </si>
   <si>
     <t>Narcissism</t>
@@ -74,9 +59,6 @@
   <si>
     <t xml:space="preserve">It seems self-evident that you deserve to have all those lovely things, certainly more than anyone else deserves them. And why not? You worked hard to get where you are!
 </t>
-  </si>
-  <si>
-    <t>You do not win the game as normal. Instead, you win only if the investigation is complete and you have 6 or more items.</t>
   </si>
   <si>
     <r>
@@ -127,25 +109,16 @@
     <t>Misery Loves Company</t>
   </si>
   <si>
-    <t>You do not win the game as normal. Instead, you win only if the investigation is complete and one or more other investigators are Insane. Otherwise, you lose the game.</t>
-  </si>
-  <si>
     <t>•	Push (Action): Choose target monster/investigator in your space, choose destination, and determine willingness. Skip test if willing. Determine test difficulty: monsters use Brawn; investigators roll Strength and add 1 to test result. Roll Strength test. If you succeed, push target to chosen space. You may also move to that space.</t>
   </si>
   <si>
     <t>Schadenfreude</t>
   </si>
   <si>
-    <t>You do not win the game as normal. Instead, you win only if the investigation is complete and one or more other investigators are Wounded. Otherwise, you lose the game.</t>
-  </si>
-  <si>
     <t>Obsessive</t>
   </si>
   <si>
     <t>You must find it. You do not know what it is, but when you see it, you will know and finally have some peace.</t>
-  </si>
-  <si>
-    <t>You do not win the game as normal. Instead, you win only if the investigation is complete and there are no Search tokens on the board. Otherwise, you lose the game.</t>
   </si>
   <si>
     <t>•	Search tokens are question marks:    ?
@@ -155,16 +128,10 @@
     <t>Restless Anxiety</t>
   </si>
   <si>
-    <t>You cannot perform any single action more than once each round. You win or lose the game as normal.</t>
-  </si>
-  <si>
     <t>You may still perform 2 actions each round, but they must each be different actions.</t>
   </si>
   <si>
     <t>Suspicious</t>
-  </si>
-  <si>
-    <t>No effect. You win or lose the game as normal.</t>
   </si>
   <si>
     <t>Your friends glance at you, distrust in their eyes.</t>
@@ -189,9 +156,6 @@
     <t>Regular weapons are useless against the powers that are aligned against you. The only thing that can keep you safe from otherworldly harm is otherworldly protection.</t>
   </si>
   <si>
-    <t>You do not win the game as normal. Instead, you win only if the investigation is complete and you have 1 or more Spells. Otherwise, you lose the game.</t>
-  </si>
-  <si>
     <t>•	Steal (Action): Pick an investigator in your space. Pick Strength, Agility, or Observation. Each player rolls that test. For each net success over your opponent’s, you take one possession. (Spells are possessions)</t>
   </si>
   <si>
@@ -201,18 +165,12 @@
     <t>The common rabble do not deserve such power, but your devotion is unquestionable.</t>
   </si>
   <si>
-    <t>You do not win the game as normal. Instead, you win only if the investigation is complete and you have more Spells than the investigator to your right. Otherwise, you lose the game.</t>
-  </si>
-  <si>
     <t>Calculating</t>
   </si>
   <si>
     <t>Trust in your companions is unnecessary. This proof will be your Insurance.</t>
   </si>
   <si>
-    <t>You do not win the game as normal. Instead, you win only if the investigation is complete and you have more Evidence than the investigator to your right. Otherwise, you lose the game.</t>
-  </si>
-  <si>
     <t>•	Steal (Action): Pick an investigator in your space. Pick Strength, Agility, or Observation. Each player rolls that test. For each net success over your opponent’s, you take one possession.</t>
   </si>
   <si>
@@ -220,9 +178,6 @@
   </si>
   <si>
     <t>The sight of other people having more than you is unacceptable. Everything should be yours.</t>
-  </si>
-  <si>
-    <t>You do not win the game as normal. Instead, you win only if the investigation is complete and you have more Items than the investigator to your left. Otherwise, you lose the game.</t>
   </si>
   <si>
     <t>•	Steal (Action): Pick an investigator in your space. Pick Strength, Agility, or Observation. Each player rolls that test. For each net success over your opponent’s, you take one possession.
@@ -235,13 +190,7 @@
     <t>You know now that anything can go wrong at any moment. Without the proper tools, all might be lost.</t>
   </si>
   <si>
-    <t>You do not win the game as normal. Instead, you win only if the investigation is complete and you have 1 or more Bladed Weapons or Light Sources.</t>
-  </si>
-  <si>
     <t>Passive</t>
-  </si>
-  <si>
-    <t>You cannot use Actions defined on your character sheet. You win or lose the game as normal.</t>
   </si>
   <si>
     <t>•	Other non-Action character abilities take place normally (such as gaining extra clues when searching, etc).
@@ -269,39 +218,81 @@
     <t>You are suddenly stricken with the sense that your life up to this point has been not only boring but pointless. Life is too short to not experience as much of the world as possible.</t>
   </si>
   <si>
-    <t>You do not win the game as normal. Instead, you win only if the investigation is complete and this card has been revealed.
-&lt;p&gt;
-&lt;b&gt;Execution Attempt:&lt;/b&gt; At the start of the Investigator Phase, if you have a Bladed Weapon and you are in a space with exactly one other investigator, you may reveal this card. If that investigator is not Wounded, he becomes Wounded and discards all facedown Damage. If he is Wounded, that investigator is eliminated. The game does not end as a result of that investigator’s elimination. This execution attempt may only happen once per game.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You do not win the game as normal. Instead, you only win if the investigation is complete and this card has been revealed.
-&lt;p&gt;
-&lt;b&gt;Conflagration:&lt;/b&gt; At the start of the Investigator Phase, if 6 or more rooms contain Fire, reveal this card. While this card is revealed, at the beginning of each Mythos phase, fire spreads twice.
-</t>
-  </si>
-  <si>
-    <t>You do not win the game as normal. Instead, you win only if the investigation is complete and this card has been revealed.
-&lt;p&gt;
-&lt;b&gt;Martyrdom:&lt;/b&gt; After you have been eliminated, reveal this card. The game does not end as a result of your elimination.</t>
-  </si>
-  <si>
-    <t>You do not win the game as normal. Instead, you win only if the investigation is complete and this card has been revealed.
-&lt;p&gt;
-&lt;b&gt;Bloodletting:&lt;/b&gt; At the start of the Investigator Phase, if you have a Bladed Weapon and there is at least one other investigator on your space, you may reveal this card and choose one investigator on your space. That investigator suffers one facedown Damage, and you discard one Horror. Other investigators within range flip one Horror.</t>
-  </si>
-  <si>
-    <t>You do not win the game as normal. Instead, you win if the investigation is complete and this card has been revealed.
-&lt;p&gt;
-&lt;b&gt;Burn the Evidence:&lt;/b&gt; At the start of the Investigator Phase, if you possess two Evidence Unique Items while standing on or adjacent to a space that contains Fire, you may reveal this card. Discard two Evidence Unique items from your inventory.</t>
-  </si>
-  <si>
-    <t>You do not win the game as normal. Instead, you win only if the investigation is complete and this card has been revealed.
-&lt;p&gt;
-&lt;b&gt;Horrific Offering:&lt;/b&gt; At the start of the Investigator Phase, if you have a Bladed Weapon and 1 or more Spells, and there is at least one other investigator on your space, you may reveal this card and choose one investigator on your space. That investigator suffers one Damage and becomes Insane. (If the investigator was already Insane, the investigator is eliminated as normal.) This offering may only happen once per game.</t>
-  </si>
-  <si>
     <t>&lt;p&gt;You do not win the game as normal. Instead, you win only if the investigation is complete and this card has been revealed.
-&lt;/p&gt;&lt;b&gt;Miracle:&lt;/b&gt; At the start of the Investigator Phase, if you have a Light Source, a Bladed Weapon, and an Evidence Unique Item, and you are sharing a space with another investigator, you may reveal this card. That investigator may discard a Wounded or Insane condition. This miracle may only happen once per game.</t>
+&lt;/p&gt;&lt;p&gt;&lt;b&gt;Miracle:&lt;/b&gt; At the start of the Investigator Phase, if you have a Light Source, a Bladed Weapon, and an Evidence Unique Item, and you are sharing a space with another investigator, you may reveal this card. That investigator may discard a Wounded or Insane condition. This miracle may only happen once per game.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You do not win the game as normal. Instead, you win only if the investigation is complete and this card has been revealed.&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;Execution Attempt:&lt;/b&gt; At the start of the Investigator Phase, if you have a Bladed Weapon and you are in a space with exactly one other investigator, you may reveal this card. If that investigator is not Wounded, he becomes Wounded and discards all facedown Damage. If he is Wounded, that investigator is eliminated. The game does not end as a result of that investigator’s elimination. This execution attempt may only happen once per game.&lt;/p&gt;&lt;p&gt;&lt;b&gt;Steal (Action):&lt;/b&gt; Pick an investigator in your space. Pick Strength, Agility, or Observation. Each player rolls that test. For each net success over your opponent's, you take one possession.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You do not win the game as normal. Instead, you win only if the investigation is complete and you have 6 or more items.&lt;/p&gt;&lt;p&gt;&lt;em&gt;Item:&lt;/em&gt; The word "Items" is a collective term that refers to both Common Items and Unique Items. Spells are not items. (Spells and Items are possessions)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You do not win the game as normal. Instead, you only win if the investigation is complete and this card has been revealed.
+&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;Conflagration:&lt;/b&gt; At the start of the Investigator Phase, if 6 or more rooms contain Fire, reveal this card. While this card is revealed, at the beginning of each Mythos phase, fire spreads twice.&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;Set Fire (Action):&lt;/b&gt; If you have a Light Source, place a Fire in your space or an adjacent space. Select the “Set Fire” option in the app.&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;Extinguish Fire (Action):&lt;/b&gt; Test Agility. For each success, discard Fire from your space or a space you move into later during the round. Doesn't do Damage.&lt;/p&gt;
+&lt;p&gt;If group disagrees about how a fire should spread, a random investigator decides. Roll a die, draw cards, use an app, or do something else.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You do not win the game as normal. Instead, you win only if the investigation is complete and this card has been revealed.
+&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;Martyrdom:&lt;/b&gt; After you have been eliminated, reveal this card. The game does not end as a result of your elimination.&lt;/p&gt;&lt;p&gt;When eliminated, you drop all possessions onto your space and remove your figure from the board. You cannot take actions.
+&lt;/p&gt;&lt;p&gt;Normally, eliminations cause the eliminated player to lose and the group to lose after the next Investigation phase. This card overrides that rule.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You do not win the game as normal. Instead, you win only if the investigation is complete and one or more other investigators are Insane. Otherwise, you lose the game.&lt;/p&gt;&lt;p&gt;&lt;b&gt;Push (Action):&lt;/b&gt; Choose target monster/investigator in your space, choose destination, and determine willingness. Skip test if willing. Determine test difficulty: monsters use Brawn; investigators roll Strength and add 1 to test result. Roll Strength test. If you succeed, push target to chosen space. You may also move to that space.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You do not win the game as normal. Instead, you win only if the investigation is complete and there are no Search tokens on the board. Otherwise, you lose the game.&lt;/p&gt;&lt;p&gt;Search tokens are question marks:    ?&lt;/p&gt;
+&lt;p&gt;You do not need to clear the Interact, Explore, Sight, and Person tokens.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You do not win the game as normal. Instead, you win if the investigation is complete and this card has been revealed.
+&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;Burn the Evidence:&lt;/b&gt; At the start of the Investigator Phase, if you possess two Evidence Unique Items while standing on or adjacent to a space that contains Fire, you may reveal this card. Discard two Evidence Unique items from your inventory.&lt;/p&gt;&lt;p&gt;&lt;b&gt;Set Fire (Action):&lt;/b&gt; If you have a Light Source, place a Fire in your space or an adjacent space. Select the "Set Fire" option in the app.&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;Steal (Action):&lt;/b&gt; Pick an investigator in your space. Pick Strength, Agility, or Observation. Each player rolls that test. For each net success over your opponent's, you take one possession.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You do not win the game as normal. Instead, you win only if the investigation is complete and you have 1 or more Spells. Otherwise, you lose the game.&lt;/p&gt;&lt;p&gt;&lt;b&gt;Steal (Action):&lt;/b&gt; Pick an investigator in your space. Pick Strength, Agility, or Observation. Each player rolls that test. For each net success over your opponent's, you take one possession. (Spells are possessions)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You do not win the game as normal. Instead, you win only if the investigation is complete and you have more Spells than the investigator to your right. Otherwise, you lose the game.&lt;/p&gt;&lt;p&gt;&lt;b&gt;Steal (Action):&lt;/b&gt; Pick an investigator in your space. Pick Strength, Agility, or Observation. Each player rolls that test. For each net success over your opponent's, you take one possession. (Spells are possessions)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You do not win the game as normal. Instead, you win only if the investigation is complete and you have more Evidence than the investigator to your right. Otherwise, you lose the game.&lt;/p&gt;&lt;p&gt;&lt;b&gt;Steal (Action):&lt;/b&gt; Pick an investigator in your space. Pick Strength, Agility, or Observation. Each player rolls that test. For each net success over your opponent's, you take one possession.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You do not win the game as normal. Instead, you win only if the investigation is complete and you have more Items than the investigator to your left. Otherwise, you lose the game.&lt;/p&gt;&lt;p&gt;&lt;b&gt;Steal (Action):&lt;/b&gt; Pick an investigator in your space. Pick Strength, Agility, or Observation. Each player rolls that test. For each net success over your opponent's, you take one possession.&lt;/p&gt;
+&lt;p&gt;&lt;em&gt;Item:&lt;/em&gt; The word "Items" is a collective term that refers to both Common Items and Unique Items. Spells are not Items.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You do not win the game as normal. Instead, you win only if the investigation is complete and you have 1 or more Bladed Weapons or Light Sources.&lt;/p&gt;&lt;p&gt;&lt;b&gt;Steal (Action):&lt;/b&gt; Pick an investigator in your space. Pick Strength, Agility, or Observation. Each player rolls that test. For each net success over your opponent's, you take one possession.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You do not win the game as normal. Instead, you win only if the investigation is complete and this card has been revealed.
+&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;Horrific Offering:&lt;/b&gt; At the start of the Investigator Phase, if you have a Bladed Weapon and 1 or more Spells, and there is at least one other investigator on your space, you may reveal this card and choose one investigator on your space. That investigator suffers one Damage and becomes Insane. (If the investigator was already Insane, the investigator is eliminated as normal.) This offering may only happen once per game.&lt;/p&gt;&lt;p&gt;&lt;b&gt;Steal (Action):&lt;/b&gt; Pick an investigator in your space. Pick Strength, Agility, or Observation. Each player rolls that test. For each net success over your opponent's, you take one possession. (Spells are possessions)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You do not win the game as normal. Instead, you win only if the investigation is complete and this card has been revealed.
+&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;Bloodletting:&lt;/b&gt; At the start of the Investigator Phase, if you have a Bladed Weapon and there is at least one other investigator on your space, you may reveal this card and choose one investigator on your space. That investigator suffers one facedown Damage, and you discard one Horror. Other investigators within range flip one Horror.&lt;/p&gt;&lt;p&gt;&lt;b&gt;Steal (Action):&lt;/b&gt; Pick an investigator in your space. Pick Strength, Agility, or Observation. Each player rolls that test. For each net success over your opponent's, you take one possession.&lt;/p&gt;
+&lt;p&gt;&lt;em&gt;"Within Range:"&lt;/em&gt; Means up to 3 spaces away. Cannot count through walls, doors, or impassable borders, unless an effect says otherwise.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You do not win the game as normal. Instead, you win only if the investigation is complete and one or more other investigators are Wounded. Otherwise, you lose the game.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You cannot perform any single action more than once each round. You win or lose the game as normal.&lt;/p&gt;&lt;p&gt;You may still perform 2 actions each round, but they must each be different actions.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;No effect.&lt;/em&gt; You win or lose the game as normal.&lt;/p&gt;&lt;p&gt;Remember, you cannot reveal the back of your Insanity card.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You cannot use Actions defined on your character sheet. You win or lose the game as normal.&lt;/p&gt;&lt;p&gt;Other non-Action character abilities take place normally (such as gaining extra clues when searching, etc).&lt;/p&gt;&lt;p&gt;Remember, you cannot reveal the back of your insanity.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -749,7 +740,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,10 +781,10 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -804,296 +795,294 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="180" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="B5" s="2">
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="108" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="B6" s="2">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="162" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2">
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2">
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B14" s="2">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B15" s="2">
         <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B16" s="2">
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B17" s="2">
         <v>3</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B19" s="2">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B20" s="2">
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added insanity for Sanctum of Twilight
</commit_message>
<xml_diff>
--- a/mom2e_insanity.xlsx
+++ b/mom2e_insanity.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trasa\mom2e\insanity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF744E8F-3018-4CFE-9D53-699DFFABF3BA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1652DADD-F01E-48A5-B2E4-3ED0DBE135F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{3318FF81-56BE-4CC7-A916-502FDCE62A14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="82">
   <si>
     <t>Name</t>
   </si>
@@ -293,6 +293,28 @@
   </si>
   <si>
     <t>&lt;p&gt;You cannot use Actions defined on your character sheet. You win or lose the game as normal.&lt;/p&gt;&lt;p&gt;Other non-Action character abilities take place normally (such as gaining extra clues when searching, etc).&lt;/p&gt;&lt;p&gt;Remember, you cannot reveal the back of your insanity.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Silver Twilight Devotee</t>
+  </si>
+  <si>
+    <t>The Order of the Silver Twilight has need of the information and artifacts you uncover.</t>
+  </si>
+  <si>
+    <t>Aggressive</t>
+  </si>
+  <si>
+    <t>You cannot agree with these people. They insist on wasting precious time and resources. Someone has to advocate for the devil or important matters may be overlooked.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You do not win the game as normal. Instead, you win only if the investigation is complete and you have 1 or more &lt;i&gt;Bladed Weapons&lt;/i&gt; and 1 or more &lt;i&gt;Unique Items.&lt;/i&gt; Otherwise, you lose the game.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You do not win the game as normal. Instead you win only if the investigation is complete and this card has been revealed.&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;Unchained Rage:&lt;/b&gt;At the start of the Investigator Phase, if you are in a space with only one investigator and no other creatures or characters, you may reveal this card and choose that investigator. That investigator suffers one Damage. This may only happen once per game.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>It must be just  the two of you together in that space - no other investigators, monsters, other non-player characters, anybody else.</t>
   </si>
 </sst>
 </file>
@@ -736,11 +758,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC2BF15-85E0-469F-B0B7-C4AF3B1AC6A5}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,6 +1107,37 @@
         <v>36</v>
       </c>
     </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="2">
+        <v>3</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
added insanity from Horrific Journeys
</commit_message>
<xml_diff>
--- a/mom2e_insanity.xlsx
+++ b/mom2e_insanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trasa\mom2e\insanity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97A4B3E-A161-4BB0-BE3A-3F7DF3256873}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D361689E-932F-4CB6-8A7B-2270B8EB7ACF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{3318FF81-56BE-4CC7-A916-502FDCE62A14}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -193,9 +193,6 @@
   </si>
   <si>
     <t>You cannot agree with these people. They insist on wasting precious time and resources. Someone has to advocate for the devil or important matters may be overlooked.</t>
-  </si>
-  <si>
-    <t>(modified)</t>
   </si>
   <si>
     <t>&lt;p&gt;You do not win the game as normal. Instead, you only win if the investigation is complete and this card has been revealed.
@@ -264,6 +261,40 @@
 &lt;p&gt;&lt;b&gt;Kleptomania:&lt;/b&gt;At the beginning of the Investigator Phase, reveal this card. While this card is revealed, you must perform the &lt;b&gt;Envious&lt;/b&gt; event at the beginning of each Investigator Phase, including this one.&lt;/p&gt;
 &lt;p&gt;&lt;b&gt;Envious:&lt;/b&gt; Pick an investigator in your space. Pick Strength, Agility, or Observation. Each player rolls that test. For each net success over your opponent's, you take one possession.&lt;/p&gt;
 &lt;p&gt;&lt;em&gt;Item:&lt;/em&gt; The word "Items" is a collective term that refers to both Common Items and Unique Items. Spells are not Items.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Paralyzing Fear</t>
+  </si>
+  <si>
+    <t>Get close to -- that?! No! Absolutely not!</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You cannot voluntarily move into a space that contains 1 or more monsters. You win or lose the game as normal.</t>
+  </si>
+  <si>
+    <t>same as original card</t>
+  </si>
+  <si>
+    <t>Right Time, Right Place</t>
+  </si>
+  <si>
+    <t>You just want to be home.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You do not win the game as normal. Instead, you win only if the investigation is complete and you are not Lost in Time and Space. Otherwise, you lose the game.</t>
+  </si>
+  <si>
+    <t>Deep One Hybrid</t>
+  </si>
+  <si>
+    <t>Your ancestors trace back to Y'ha-nthlei and Innsmouth. They demand that you prove your worth.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You do not win the game as normal. Instead, you win only if the investigation is complete and you have 2 or more &lt;em&gt;Evidence&lt;/em&gt;.&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;Steal (Action):&lt;/b&gt; Pick an investigator in your space. Pick Strength, Agility, or Observation. Each player rolls that test. For each net success over your opponent's, you take one possession.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>removed traitor aspect - come up with something better?</t>
   </si>
 </sst>
 </file>
@@ -710,11 +741,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC2BF15-85E0-469F-B0B7-C4AF3B1AC6A5}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,7 +758,7 @@
     <col min="6" max="16384" width="27.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -744,7 +775,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -755,13 +786,10 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -772,14 +800,11 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:5" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -790,14 +815,11 @@
         <v>10</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -808,13 +830,10 @@
         <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="108" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="108" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -828,7 +847,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="162" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="162" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -839,13 +858,10 @@
         <v>15</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -859,7 +875,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -873,7 +889,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -887,7 +903,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -898,14 +914,11 @@
         <v>42</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E11"/>
-      <c r="F11" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -920,7 +933,7 @@
       </c>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -931,13 +944,10 @@
         <v>24</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -951,7 +961,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
@@ -962,13 +972,10 @@
         <v>28</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
@@ -979,10 +986,7 @@
         <v>30</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="165" x14ac:dyDescent="0.25">
@@ -996,10 +1000,7 @@
         <v>32</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1027,10 +1028,7 @@
         <v>41</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="180" x14ac:dyDescent="0.25">
@@ -1044,10 +1042,7 @@
         <v>37</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1061,10 +1056,7 @@
         <v>51</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1078,10 +1070,58 @@
         <v>53</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="2">
+        <v>3</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="2">
+        <v>3</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Path of the Serpent insanity cards
</commit_message>
<xml_diff>
--- a/mom2e_insanity.xlsx
+++ b/mom2e_insanity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trasa\mom2e\insanity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D361689E-932F-4CB6-8A7B-2270B8EB7ACF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3A1942-4687-4FAE-90EC-387EE3FC8D61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{3318FF81-56BE-4CC7-A916-502FDCE62A14}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3318FF81-56BE-4CC7-A916-502FDCE62A14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -295,6 +295,24 @@
   </si>
   <si>
     <t>removed traitor aspect - come up with something better?</t>
+  </si>
+  <si>
+    <t>Ophidiophobia</t>
+  </si>
+  <si>
+    <t>Why did it have to be snakes?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You cannot voluntarily move into a space that contains a Hunting Horror, Feathered Serpent, Serpent Person, or Ancient Basilisk. You win or lose the game as normal.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Treasure Hunter</t>
+  </si>
+  <si>
+    <t>You deserve a reward for your good work. There must be some valuables around here somewhere.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You do not win the game as normal. Instead, you win only if the investigation is complete and there are no Items on the board.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -741,11 +759,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC2BF15-85E0-469F-B0B7-C4AF3B1AC6A5}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,6 +1142,34 @@
         <v>78</v>
       </c>
     </row>
+    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="2">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>